<commit_message>
Add more tests and evaluateAll function
</commit_message>
<xml_diff>
--- a/xcelreader/excel_files/test_populate.xlsx
+++ b/xcelreader/excel_files/test_populate.xlsx
@@ -124,30 +124,38 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="B2" s="0" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="b">
+      <c r="A3" s="1" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <f aca="false">SUM(B1:B2)</f>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>